<commit_message>
Results Summary And ActionableItems
Added a new excel sheet and pdf file that summarizes the results over the two months in one document.
Added a text file with summary of the results and insights and actionable items based on them.
</commit_message>
<xml_diff>
--- a/Fitabase Data 4.12.16-5.12.16/TotalDailyActivitySummedUp_04_05_2016.xlsx
+++ b/Fitabase Data 4.12.16-5.12.16/TotalDailyActivitySummedUp_04_05_2016.xlsx
@@ -8,27 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\palla\Desktop\GoogleDataAnalyticsCapstoneProject\BellaBeatsCaseStudy\Wearable-Fitness-Tracker-Feature-Analysis\Fitabase Data 4.12.16-5.12.16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680C54DF-6A14-4B68-B078-C388104D2BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D5615A-F16E-44EA-B409-5D607467C42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PivotTable" sheetId="5" r:id="rId1"/>
     <sheet name="TotalDailyActivitySummedUp_04_0" sheetId="1" r:id="rId2"/>
-    <sheet name="FeaturesByUserPlot" sheetId="7" r:id="rId3"/>
+    <sheet name="FeaturesByIndividualUserPlot" sheetId="7" r:id="rId3"/>
     <sheet name="HeatMapOfFeatureUse" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">TotalDailyActivitySummedUp_04_0!$T$2:$W$13</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">TotalDailyActivitySummedUp_04_0!$X$2:$X$13</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">TotalDailyActivitySummedUp_04_0!$T$2:$W$13</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">TotalDailyActivitySummedUp_04_0!$X$2:$X$13</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">TotalDailyActivitySummedUp_04_0!$T$2:$W$13</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">TotalDailyActivitySummedUp_04_0!$X$2:$X$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -67,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="62">
   <si>
     <t>overall_Id</t>
   </si>
@@ -225,9 +221,6 @@
     <t>LoggedActivitiesDistance</t>
   </si>
   <si>
-    <t>From FeatureUse_03_04_2016.csv</t>
-  </si>
-  <si>
     <t>Activity + LoggedActivityDistance</t>
   </si>
   <si>
@@ -253,6 +246,9 @@
   </si>
   <si>
     <t>No HR</t>
+  </si>
+  <si>
+    <t>From FeatureUse_04_05_2016.csv</t>
   </si>
 </sst>
 </file>
@@ -980,7 +976,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1062,17 +1058,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1085,9 +1072,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1116,6 +1100,15 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1247,7 +1240,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1273,27 +1266,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$3:$N$3</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$3:$N$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.453903433219203</c:v>
+                  <c:v>31.461473022984936</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.186355832676476</c:v>
+                  <c:v>25.052259078047523</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4448547237597964</c:v>
+                  <c:v>2.0555363392228245</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1139835195807688</c:v>
+                  <c:v>1.0637770797426032</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1332,7 +1325,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1358,12 +1351,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$4:$N$4</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$4:$N$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.279102147024648</c:v>
+                  <c:v>31.200607688529882</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -1417,7 +1410,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1443,18 +1436,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$5:$N$5</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$5:$N$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>30.262978294277076</c:v>
+                  <c:v>30.3632133755642</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.2887257285601823</c:v>
+                  <c:v>4.4054876933432485</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -1502,7 +1495,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1528,18 +1521,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$6:$N$6</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$6:$N$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.372742432549778</c:v>
+                  <c:v>31.168244203912469</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.4818107010679515</c:v>
+                  <c:v>3.2618977337722663</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -1587,7 +1580,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1613,24 +1606,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$7:$N$7</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$7:$N$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.430891888308167</c:v>
+                  <c:v>31.417958691966508</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.3282325277604867</c:v>
+                  <c:v>5.2143170936440448</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0149340957892918</c:v>
+                  <c:v>1.2231611204392672</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>#N/A</c:v>
@@ -1672,7 +1665,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1698,12 +1691,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$8:$N$8</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$8:$N$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.496294534748667</c:v>
+                  <c:v>31.012793319418492</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -1712,7 +1705,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.34258830447531</c:v>
+                  <c:v>31.016614485613424</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
@@ -1761,7 +1754,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1787,21 +1780,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$9:$N$9</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$9:$N$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.3555634313397</c:v>
+                  <c:v>31.069141519983937</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.003571193387174</c:v>
+                  <c:v>28.076331412787258</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.4995204488810003</c:v>
+                  <c:v>4.4115887112533061</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
@@ -1850,7 +1843,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1876,18 +1869,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$10:$N$10</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$10:$N$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.216915793599973</c:v>
+                  <c:v>31.084064572201765</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0762387895731864</c:v>
+                  <c:v>1.4543454798042026</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -1939,7 +1932,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1965,21 +1958,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$11:$N$11</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$11:$N$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>18.458082302148149</c:v>
+                  <c:v>18.039200524699414</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.162213570459105</c:v>
+                  <c:v>15.293799731838</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.213338461946048</c:v>
+                  <c:v>18.430707457479613</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
@@ -2028,7 +2021,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2054,12 +2047,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$12:$N$12</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$12:$N$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.093058509138924</c:v>
+                  <c:v>31.048537580178518</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -2071,7 +2064,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4904864352782092</c:v>
+                  <c:v>2.2259736836119153</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>#N/A</c:v>
@@ -2117,7 +2110,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2143,12 +2136,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$13:$N$13</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$13:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>20.345134375427005</c:v>
+                  <c:v>20.472515807659121</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -2206,7 +2199,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2232,18 +2225,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$14:$N$14</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$14:$N$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>30.066097012792149</c:v>
+                  <c:v>30.157448268500492</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.320032432274161</c:v>
+                  <c:v>28.204713442580633</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -2297,7 +2290,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2323,21 +2316,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$15:$N$15</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$15:$N$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.120431545440891</c:v>
+                  <c:v>31.416831024138872</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.3144738602731341</c:v>
+                  <c:v>8.4530250686686248</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.304689349326676</c:v>
+                  <c:v>16.231085208066578</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
@@ -2388,7 +2381,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2414,12 +2407,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$16:$N$16</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$16:$N$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.2950394269361505</c:v>
+                  <c:v>4.4181102579559068</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -2479,7 +2472,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2505,27 +2498,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$17:$N$17</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$17:$N$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.262765653713338</c:v>
+                  <c:v>31.462421172100999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.185310916732359</c:v>
+                  <c:v>26.123524506294977</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0471731212423023</c:v>
+                  <c:v>2.3614127775548104</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0356155504670561</c:v>
+                  <c:v>1.3977016490040139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2570,7 +2563,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2596,21 +2589,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$18:$N$18</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$18:$N$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.147550301393355</c:v>
+                  <c:v>31.440367940564144</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.467449682996154</c:v>
+                  <c:v>23.376552979336282</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.080857493239282</c:v>
+                  <c:v>30.091086646681312</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
@@ -2661,7 +2654,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2687,18 +2680,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$19:$N$19</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$19:$N$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.252320625645694</c:v>
+                  <c:v>31.369249548056697</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.378891217076628</c:v>
+                  <c:v>28.089247940355147</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -2752,7 +2745,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2778,24 +2771,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$20:$N$20</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$20:$N$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.485415094953346</c:v>
+                  <c:v>31.445192654801264</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1317677509213624</c:v>
+                  <c:v>5.2472909191075097</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.366307824210971</c:v>
+                  <c:v>31.379103193205228</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.322742297855771</c:v>
+                  <c:v>5.4674717289577455</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>#N/A</c:v>
@@ -2841,7 +2834,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2867,18 +2860,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$21:$N$21</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$21:$N$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.207700742323802</c:v>
+                  <c:v>31.456405441568453</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.045082052367427</c:v>
+                  <c:v>27.355210351759897</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -2930,7 +2923,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2956,21 +2949,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$22:$N$22</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$22:$N$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.34061826007833</c:v>
+                  <c:v>31.467108007794707</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.145459684140935</c:v>
+                  <c:v>31.492323553978618</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.291215195525034</c:v>
+                  <c:v>31.330967765232845</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
@@ -3019,7 +3012,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -3045,24 +3038,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$23:$N$23</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$23:$N$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>30.096729792249217</c:v>
+                  <c:v>30.279329563698237</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.159040864306363</c:v>
+                  <c:v>26.219795097284894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.233459647030408</c:v>
+                  <c:v>28.112245651755075</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3637677535953165</c:v>
+                  <c:v>1.0339136295808249</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>#N/A</c:v>
@@ -3108,7 +3101,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -3134,21 +3127,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$24:$N$24</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$24:$N$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>28.086806403832227</c:v>
+                  <c:v>28.465298296367251</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.252188461107949</c:v>
+                  <c:v>18.031123959078641</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.482486930823775</c:v>
+                  <c:v>23.477982785817609</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
@@ -3197,7 +3190,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -3223,12 +3216,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$25:$N$25</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$25:$N$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>29.373369342383853</c:v>
+                  <c:v>29.152605492027078</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -3286,7 +3279,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -3312,21 +3305,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$26:$N$26</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$26:$N$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>26.364594825834761</c:v>
+                  <c:v>26.441229928225766</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1086203324922375</c:v>
+                  <c:v>1.0862740533764064</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.3554119889312726</c:v>
+                  <c:v>3.1012290839292027</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.098844549609321</c:v>
+                  <c:v>18.368049572155442</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
@@ -3377,7 +3370,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -3403,24 +3396,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$27:$N$27</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$27:$N$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.322523796878709</c:v>
+                  <c:v>31.06776754107883</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2863093947018265</c:v>
+                  <c:v>3.1545694694569439</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.315025932943279</c:v>
+                  <c:v>31.205346936651591</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.49384080281181</c:v>
+                  <c:v>31.337223247045571</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.208225990418402</c:v>
+                  <c:v>30.488210193683983</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>#N/A</c:v>
@@ -3468,7 +3461,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -3494,21 +3487,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$28:$N$28</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$28:$N$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>26.036942692492595</c:v>
+                  <c:v>26.138725705630371</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.272374383789597</c:v>
+                  <c:v>12.43685809570859</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4456348089841082</c:v>
+                  <c:v>2.3419397129491037</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.300379063965124</c:v>
+                  <c:v>24.114409142835832</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
@@ -3559,7 +3552,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -3585,18 +3578,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$29:$N$29</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$29:$N$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.207941650955885</c:v>
+                  <c:v>31.050714405600107</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.460683513794638</c:v>
+                  <c:v>24.460721535470892</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -3650,7 +3643,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -3676,18 +3669,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$30:$N$30</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$30:$N$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.279108116327787</c:v>
+                  <c:v>31.199354490885145</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.272083564260468</c:v>
+                  <c:v>3.3481777610121606</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -3741,7 +3734,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -3767,12 +3760,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$31:$N$31</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$31:$N$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>19.401169814586368</c:v>
+                  <c:v>19.158111593861499</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -3832,7 +3825,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -3858,18 +3851,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$32:$N$32</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$32:$N$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.351263915361923</c:v>
+                  <c:v>31.439357081533554</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.352985599826461</c:v>
+                  <c:v>16.317198288191733</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.255659209738887</c:v>
+                  <c:v>31.060873735585556</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -3921,7 +3914,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -3947,12 +3940,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$33:$N$33</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$33:$N$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.339769137303353</c:v>
+                  <c:v>31.467372477214536</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -4010,7 +4003,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -4036,21 +4029,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$34:$N$34</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$34:$N$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>29.125343932455021</c:v>
+                  <c:v>29.279239435850442</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.166878785367489</c:v>
+                  <c:v>15.117989060446702</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.005857944050817</c:v>
+                  <c:v>18.084431201653999</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
@@ -4099,7 +4092,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$I$2:$N$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$2:$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -4125,12 +4118,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$I$35:$N$35</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$I$35:$N$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.32400601742998</c:v>
+                  <c:v>31.102067177685047</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>#N/A</c:v>
@@ -4139,10 +4132,10 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.259716430408627</c:v>
+                  <c:v>31.409788815201715</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.086040676067817</c:v>
+                  <c:v>24.182463286258006</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>#N/A</c:v>
@@ -4270,7 +4263,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Number of times a metric was logged</a:t>
+                  <a:t>Number of logs</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4472,7 +4465,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$B$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4496,7 +4489,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$B$3:$B$35</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$B$3:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
@@ -4613,7 +4606,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$D$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4640,7 +4633,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$D$3:$D$35</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$D$3:$D$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
@@ -4757,7 +4750,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$E$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4781,7 +4774,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$E$3:$E$35</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$E$3:$E$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
@@ -4898,7 +4891,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$C$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4920,7 +4913,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$C$3:$C$35</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$C$3:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
@@ -5037,7 +5030,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$F$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5065,7 +5058,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$F$3:$F$35</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$F$3:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
@@ -5182,7 +5175,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>FeaturesByUserPlot!$G$2</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5205,7 +5198,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>FeaturesByUserPlot!$G$3:$G$35</c:f>
+              <c:f>FeaturesByIndividualUserPlot!$G$3:$G$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="33"/>
@@ -5483,7 +5476,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Number of times a metric was logged</a:t>
+                  <a:t>Number of logs</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5641,10 +5634,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -7630,7 +7623,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="18768244" y="4701038"/>
+              <a:off x="18768244" y="4519005"/>
               <a:ext cx="12249389" cy="12297206"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -7917,7 +7910,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable29" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable29" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -8488,8 +8481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="37" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AE65" sqref="AE65"/>
+    <sheetView topLeftCell="F1" zoomScale="57" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -8505,19 +8498,19 @@
     <col min="21" max="21" width="21.29296875" style="3" customWidth="1"/>
     <col min="22" max="22" width="18.46875" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="18.46875" style="3" customWidth="1"/>
-    <col min="24" max="24" width="18.234375" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.703125" style="3" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="20.5859375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10.52734375" customWidth="1"/>
     <col min="29" max="29" width="7.76171875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="28.1171875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="36.234375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="36.1171875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="2.76171875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="5.234375" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="18.703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="4" customFormat="1" ht="57.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:33" s="4" customFormat="1" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -8569,19 +8562,19 @@
       <c r="R1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="42" t="s">
+      <c r="T1" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="43" t="s">
+      <c r="U1" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="43" t="s">
+      <c r="V1" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="43" t="s">
+      <c r="W1" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="X1" s="43" t="s">
+      <c r="X1" s="40" t="s">
         <v>26</v>
       </c>
       <c r="Y1" s="44"/>
@@ -8589,10 +8582,10 @@
         <v>30</v>
       </c>
       <c r="AE1" s="4" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1503960366</v>
       </c>
@@ -8649,18 +8642,18 @@
         <v>27</v>
       </c>
       <c r="U2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="V2" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="V2" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="W2" s="8"/>
-      <c r="X2" s="10">
-        <f t="shared" ref="X2:X13" si="0">Y2/$Y$14</f>
+      <c r="W2" s="45"/>
+      <c r="X2" s="9">
+        <v>6</v>
+      </c>
+      <c r="Y2" s="10">
+        <f t="shared" ref="Y2:Y12" si="0">X2/$X$14</f>
         <v>0.18181818181818182</v>
-      </c>
-      <c r="Y2" s="9">
-        <v>6</v>
       </c>
       <c r="AA2" s="4" t="s">
         <v>29</v>
@@ -8731,16 +8724,16 @@
       </c>
       <c r="T3" s="26"/>
       <c r="U3" s="7"/>
-      <c r="V3" s="34"/>
+      <c r="V3" s="31"/>
       <c r="W3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="X3" s="32">
+      <c r="X3" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="10">
         <f t="shared" si="0"/>
         <v>3.0303030303030304E-2</v>
-      </c>
-      <c r="Y3" s="14">
-        <v>1</v>
       </c>
       <c r="AA3" t="s">
         <v>17</v>
@@ -8822,18 +8815,18 @@
         <v>19</v>
       </c>
       <c r="W4" s="16"/>
-      <c r="X4" s="31">
+      <c r="X4" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="10">
         <f t="shared" si="0"/>
         <v>3.0303030303030304E-2</v>
       </c>
-      <c r="Y4" s="17">
-        <v>1</v>
-      </c>
       <c r="AA4" t="s">
         <v>51</v>
       </c>
       <c r="AB4">
-        <f>SUM(Y11:Y13)</f>
+        <f>SUM(X11:X13)</f>
         <v>4</v>
       </c>
       <c r="AC4" s="5">
@@ -8906,22 +8899,22 @@
       </c>
       <c r="T5" s="27"/>
       <c r="U5" s="12"/>
-      <c r="V5" s="33"/>
+      <c r="V5" s="30"/>
       <c r="W5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="X5" s="32">
+      <c r="X5" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="10">
         <f t="shared" si="0"/>
         <v>3.0303030303030304E-2</v>
       </c>
-      <c r="Y5" s="14">
-        <v>1</v>
-      </c>
       <c r="AA5" t="s">
         <v>18</v>
       </c>
       <c r="AB5">
-        <f>SUM(Y6:Y13)</f>
+        <f>SUM(X6:X13)</f>
         <v>24</v>
       </c>
       <c r="AC5" s="5">
@@ -8996,22 +8989,22 @@
       <c r="U6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="V6" s="30" t="s">
-        <v>61</v>
+      <c r="V6" s="29" t="s">
+        <v>60</v>
       </c>
       <c r="W6" s="16"/>
-      <c r="X6" s="31">
+      <c r="X6" s="17">
+        <v>8</v>
+      </c>
+      <c r="Y6" s="10">
         <f t="shared" si="0"/>
         <v>0.24242424242424243</v>
       </c>
-      <c r="Y6" s="17">
-        <v>8</v>
-      </c>
       <c r="AA6" t="s">
         <v>19</v>
       </c>
       <c r="AB6">
-        <f>SUM(Y4:Y5,Y9:Y10,Y12:Y13)</f>
+        <f>SUM(X4:X5,X9:X10,X12:X13)</f>
         <v>14</v>
       </c>
       <c r="AC6" s="5">
@@ -9085,21 +9078,21 @@
       <c r="T7" s="27"/>
       <c r="U7" s="18"/>
       <c r="V7" s="22"/>
-      <c r="W7" s="6" t="s">
+      <c r="W7" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="X7" s="10">
+      <c r="X7" s="9">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="10">
         <f t="shared" si="0"/>
         <v>3.0303030303030304E-2</v>
       </c>
-      <c r="Y7" s="9">
-        <v>1</v>
-      </c>
       <c r="AA7" t="s">
         <v>25</v>
       </c>
       <c r="AB7">
-        <f>SUM(Y3,Y5,Y7:Y8,Y10,Y13)</f>
+        <f>SUM(X3,X5,X7:X8,X10,X13)</f>
         <v>8</v>
       </c>
       <c r="AC7" s="5">
@@ -9176,12 +9169,12 @@
       <c r="W8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="X8" s="32">
+      <c r="X8" s="14">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="10">
         <f t="shared" si="0"/>
         <v>6.0606060606060608E-2</v>
-      </c>
-      <c r="Y8" s="14">
-        <v>2</v>
       </c>
       <c r="AE8" t="s">
         <v>37</v>
@@ -9253,12 +9246,12 @@
         <v>19</v>
       </c>
       <c r="W9" s="23"/>
-      <c r="X9" s="31">
+      <c r="X9" s="17">
+        <v>7</v>
+      </c>
+      <c r="Y9" s="10">
         <f t="shared" si="0"/>
         <v>0.21212121212121213</v>
-      </c>
-      <c r="Y9" s="17">
-        <v>7</v>
       </c>
       <c r="AE9" t="s">
         <v>38</v>
@@ -9330,12 +9323,12 @@
       <c r="W10" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="X10" s="29">
+      <c r="X10" s="21">
+        <v>2</v>
+      </c>
+      <c r="Y10" s="10">
         <f t="shared" si="0"/>
         <v>6.0606060606060608E-2</v>
-      </c>
-      <c r="Y10" s="21">
-        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:33" ht="71.7" x14ac:dyDescent="0.5">
@@ -9392,21 +9385,21 @@
         <v>A____Wt_M__</v>
       </c>
       <c r="T11" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="U11" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="U11" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="V11" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="W11" s="36"/>
-      <c r="X11" s="37">
+      <c r="V11" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="W11" s="33"/>
+      <c r="X11" s="34">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="10">
         <f t="shared" si="0"/>
         <v>3.0303030303030304E-2</v>
-      </c>
-      <c r="Y11" s="38">
-        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.5">
@@ -9463,17 +9456,17 @@
         <v>A_______</v>
       </c>
       <c r="T12" s="27"/>
-      <c r="U12" s="40"/>
+      <c r="U12" s="36"/>
       <c r="V12" s="15" t="s">
         <v>19</v>
       </c>
       <c r="W12" s="23"/>
-      <c r="X12" s="31">
+      <c r="X12" s="17">
+        <v>2</v>
+      </c>
+      <c r="Y12" s="10">
         <f t="shared" si="0"/>
         <v>6.0606060606060608E-2</v>
-      </c>
-      <c r="Y12" s="17">
-        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:33" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -9530,17 +9523,17 @@
         <v>A__Sl_____</v>
       </c>
       <c r="T13" s="28"/>
-      <c r="U13" s="41"/>
-      <c r="V13" s="35"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="32"/>
       <c r="W13" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="X13" s="29">
-        <f t="shared" si="0"/>
+      <c r="X13" s="21">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="10">
+        <f>X13/$X$14</f>
         <v>3.0303030303030304E-2</v>
-      </c>
-      <c r="Y13" s="21">
-        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.5">
@@ -9599,9 +9592,8 @@
       <c r="T14" s="6"/>
       <c r="U14" s="25"/>
       <c r="V14" s="25"/>
-      <c r="X14" s="5"/>
-      <c r="Y14">
-        <f>SUM(Y2:Y13)</f>
+      <c r="X14">
+        <f>SUM(X2:X13)</f>
         <v>33</v>
       </c>
     </row>
@@ -10714,8 +10706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D73A1E79-31F3-48A4-8129-C8985EBFF307}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" topLeftCell="J8" zoomScale="76" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -10735,14 +10727,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.5">
-      <c r="I1" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
+      <c r="I1" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
@@ -10752,7 +10744,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -10761,16 +10753,16 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K2" t="s">
         <v>18</v>
@@ -10779,10 +10771,10 @@
         <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.5">
@@ -10809,7 +10801,7 @@
       </c>
       <c r="I3" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">_xlfn.SWITCH(B3,0,NA(),B3+(RAND()*0.5))</f>
-        <v>31.453903433219203</v>
+        <v>31.461473022984936</v>
       </c>
       <c r="J3" t="e" cm="1">
         <f t="array" aca="1" ref="J3" ca="1">_xlfn.SWITCH(C3,0,NA(),C3+(RAND()*0.5))</f>
@@ -10817,7 +10809,7 @@
       </c>
       <c r="K3" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">_xlfn.SWITCH(D3,0,NA(),D3+(RAND()*0.5))</f>
-        <v>25.186355832676476</v>
+        <v>25.052259078047523</v>
       </c>
       <c r="L3" t="e" cm="1">
         <f t="array" aca="1" ref="L3" ca="1">_xlfn.SWITCH(E3,0,NA(),E3+(RAND()*0.5))</f>
@@ -10825,11 +10817,11 @@
       </c>
       <c r="M3" cm="1">
         <f t="array" aca="1" ref="M3" ca="1">_xlfn.SWITCH(F3,0,NA(),F3+(RAND()*0.5))</f>
-        <v>2.4448547237597964</v>
+        <v>2.0555363392228245</v>
       </c>
       <c r="N3" cm="1">
         <f t="array" aca="1" ref="N3" ca="1">_xlfn.SWITCH(G3,0,NA(),G3+(RAND()*0.5))</f>
-        <v>1.1139835195807688</v>
+        <v>1.0637770797426032</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.5">
@@ -10856,7 +10848,7 @@
       </c>
       <c r="I4" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">_xlfn.SWITCH(B4,0,NA(),B4+(RAND()*0.5))</f>
-        <v>31.279102147024648</v>
+        <v>31.200607688529882</v>
       </c>
       <c r="J4" t="e" cm="1">
         <f t="array" aca="1" ref="J4" ca="1">_xlfn.SWITCH(C4,0,NA(),C4+(RAND()*0.5))</f>
@@ -10903,7 +10895,7 @@
       </c>
       <c r="I5" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">_xlfn.SWITCH(B5,0,NA(),B5+(RAND()*0.5))</f>
-        <v>30.262978294277076</v>
+        <v>30.3632133755642</v>
       </c>
       <c r="J5" t="e" cm="1">
         <f t="array" aca="1" ref="J5" ca="1">_xlfn.SWITCH(C5,0,NA(),C5+(RAND()*0.5))</f>
@@ -10911,7 +10903,7 @@
       </c>
       <c r="K5" cm="1">
         <f t="array" aca="1" ref="K5" ca="1">_xlfn.SWITCH(D5,0,NA(),D5+(RAND()*0.5))</f>
-        <v>4.2887257285601823</v>
+        <v>4.4054876933432485</v>
       </c>
       <c r="L5" t="e" cm="1">
         <f t="array" aca="1" ref="L5" ca="1">_xlfn.SWITCH(E5,0,NA(),E5+(RAND()*0.5))</f>
@@ -10950,7 +10942,7 @@
       </c>
       <c r="I6" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">_xlfn.SWITCH(B6,0,NA(),B6+(RAND()*0.5))</f>
-        <v>31.372742432549778</v>
+        <v>31.168244203912469</v>
       </c>
       <c r="J6" t="e" cm="1">
         <f t="array" aca="1" ref="J6" ca="1">_xlfn.SWITCH(C6,0,NA(),C6+(RAND()*0.5))</f>
@@ -10958,7 +10950,7 @@
       </c>
       <c r="K6" cm="1">
         <f t="array" aca="1" ref="K6" ca="1">_xlfn.SWITCH(D6,0,NA(),D6+(RAND()*0.5))</f>
-        <v>3.4818107010679515</v>
+        <v>3.2618977337722663</v>
       </c>
       <c r="L6" t="e" cm="1">
         <f t="array" aca="1" ref="L6" ca="1">_xlfn.SWITCH(E6,0,NA(),E6+(RAND()*0.5))</f>
@@ -10997,7 +10989,7 @@
       </c>
       <c r="I7" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_xlfn.SWITCH(B7,0,NA(),B7+(RAND()*0.5))</f>
-        <v>31.430891888308167</v>
+        <v>31.417958691966508</v>
       </c>
       <c r="J7" t="e" cm="1">
         <f t="array" aca="1" ref="J7" ca="1">_xlfn.SWITCH(C7,0,NA(),C7+(RAND()*0.5))</f>
@@ -11005,7 +10997,7 @@
       </c>
       <c r="K7" cm="1">
         <f t="array" aca="1" ref="K7" ca="1">_xlfn.SWITCH(D7,0,NA(),D7+(RAND()*0.5))</f>
-        <v>5.3282325277604867</v>
+        <v>5.2143170936440448</v>
       </c>
       <c r="L7" t="e" cm="1">
         <f t="array" aca="1" ref="L7" ca="1">_xlfn.SWITCH(E7,0,NA(),E7+(RAND()*0.5))</f>
@@ -11013,7 +11005,7 @@
       </c>
       <c r="M7" cm="1">
         <f t="array" aca="1" ref="M7" ca="1">_xlfn.SWITCH(F7,0,NA(),F7+(RAND()*0.5))</f>
-        <v>1.0149340957892918</v>
+        <v>1.2231611204392672</v>
       </c>
       <c r="N7" t="e" cm="1">
         <f t="array" aca="1" ref="N7" ca="1">_xlfn.SWITCH(G7,0,NA(),G7+(RAND()*0.5))</f>
@@ -11044,7 +11036,7 @@
       </c>
       <c r="I8" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_xlfn.SWITCH(B8,0,NA(),B8+(RAND()*0.5))</f>
-        <v>31.496294534748667</v>
+        <v>31.012793319418492</v>
       </c>
       <c r="J8" t="e" cm="1">
         <f t="array" aca="1" ref="J8" ca="1">_xlfn.SWITCH(C8,0,NA(),C8+(RAND()*0.5))</f>
@@ -11056,7 +11048,7 @@
       </c>
       <c r="L8" cm="1">
         <f t="array" aca="1" ref="L8" ca="1">_xlfn.SWITCH(E8,0,NA(),E8+(RAND()*0.5))</f>
-        <v>31.34258830447531</v>
+        <v>31.016614485613424</v>
       </c>
       <c r="M8" t="e" cm="1">
         <f t="array" aca="1" ref="M8" ca="1">_xlfn.SWITCH(F8,0,NA(),F8+(RAND()*0.5))</f>
@@ -11091,7 +11083,7 @@
       </c>
       <c r="I9" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_xlfn.SWITCH(B9,0,NA(),B9+(RAND()*0.5))</f>
-        <v>31.3555634313397</v>
+        <v>31.069141519983937</v>
       </c>
       <c r="J9" t="e" cm="1">
         <f t="array" aca="1" ref="J9" ca="1">_xlfn.SWITCH(C9,0,NA(),C9+(RAND()*0.5))</f>
@@ -11099,11 +11091,11 @@
       </c>
       <c r="K9" cm="1">
         <f t="array" aca="1" ref="K9" ca="1">_xlfn.SWITCH(D9,0,NA(),D9+(RAND()*0.5))</f>
-        <v>28.003571193387174</v>
+        <v>28.076331412787258</v>
       </c>
       <c r="L9" cm="1">
         <f t="array" aca="1" ref="L9" ca="1">_xlfn.SWITCH(E9,0,NA(),E9+(RAND()*0.5))</f>
-        <v>4.4995204488810003</v>
+        <v>4.4115887112533061</v>
       </c>
       <c r="M9" t="e" cm="1">
         <f t="array" aca="1" ref="M9" ca="1">_xlfn.SWITCH(F9,0,NA(),F9+(RAND()*0.5))</f>
@@ -11138,7 +11130,7 @@
       </c>
       <c r="I10" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">_xlfn.SWITCH(B10,0,NA(),B10+(RAND()*0.5))</f>
-        <v>31.216915793599973</v>
+        <v>31.084064572201765</v>
       </c>
       <c r="J10" t="e" cm="1">
         <f t="array" aca="1" ref="J10" ca="1">_xlfn.SWITCH(C10,0,NA(),C10+(RAND()*0.5))</f>
@@ -11146,7 +11138,7 @@
       </c>
       <c r="K10" cm="1">
         <f t="array" aca="1" ref="K10" ca="1">_xlfn.SWITCH(D10,0,NA(),D10+(RAND()*0.5))</f>
-        <v>1.0762387895731864</v>
+        <v>1.4543454798042026</v>
       </c>
       <c r="L10" t="e" cm="1">
         <f t="array" aca="1" ref="L10" ca="1">_xlfn.SWITCH(E10,0,NA(),E10+(RAND()*0.5))</f>
@@ -11185,7 +11177,7 @@
       </c>
       <c r="I11" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_xlfn.SWITCH(B11,0,NA(),B11+(RAND()*0.5))</f>
-        <v>18.458082302148149</v>
+        <v>18.039200524699414</v>
       </c>
       <c r="J11" t="e" cm="1">
         <f t="array" aca="1" ref="J11" ca="1">_xlfn.SWITCH(C11,0,NA(),C11+(RAND()*0.5))</f>
@@ -11193,11 +11185,11 @@
       </c>
       <c r="K11" cm="1">
         <f t="array" aca="1" ref="K11" ca="1">_xlfn.SWITCH(D11,0,NA(),D11+(RAND()*0.5))</f>
-        <v>15.162213570459105</v>
+        <v>15.293799731838</v>
       </c>
       <c r="L11" cm="1">
         <f t="array" aca="1" ref="L11" ca="1">_xlfn.SWITCH(E11,0,NA(),E11+(RAND()*0.5))</f>
-        <v>18.213338461946048</v>
+        <v>18.430707457479613</v>
       </c>
       <c r="M11" t="e" cm="1">
         <f t="array" aca="1" ref="M11" ca="1">_xlfn.SWITCH(F11,0,NA(),F11+(RAND()*0.5))</f>
@@ -11232,7 +11224,7 @@
       </c>
       <c r="I12" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">_xlfn.SWITCH(B12,0,NA(),B12+(RAND()*0.5))</f>
-        <v>31.093058509138924</v>
+        <v>31.048537580178518</v>
       </c>
       <c r="J12" t="e" cm="1">
         <f t="array" aca="1" ref="J12" ca="1">_xlfn.SWITCH(C12,0,NA(),C12+(RAND()*0.5))</f>
@@ -11248,7 +11240,7 @@
       </c>
       <c r="M12" cm="1">
         <f t="array" aca="1" ref="M12" ca="1">_xlfn.SWITCH(F12,0,NA(),F12+(RAND()*0.5))</f>
-        <v>2.4904864352782092</v>
+        <v>2.2259736836119153</v>
       </c>
       <c r="N12" t="e" cm="1">
         <f t="array" aca="1" ref="N12" ca="1">_xlfn.SWITCH(G12,0,NA(),G12+(RAND()*0.5))</f>
@@ -11279,7 +11271,7 @@
       </c>
       <c r="I13" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">_xlfn.SWITCH(B13,0,NA(),B13+(RAND()*0.5))</f>
-        <v>20.345134375427005</v>
+        <v>20.472515807659121</v>
       </c>
       <c r="J13" t="e" cm="1">
         <f t="array" aca="1" ref="J13" ca="1">_xlfn.SWITCH(C13,0,NA(),C13+(RAND()*0.5))</f>
@@ -11326,7 +11318,7 @@
       </c>
       <c r="I14" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">_xlfn.SWITCH(B14,0,NA(),B14+(RAND()*0.5))</f>
-        <v>30.066097012792149</v>
+        <v>30.157448268500492</v>
       </c>
       <c r="J14" t="e" cm="1">
         <f t="array" aca="1" ref="J14" ca="1">_xlfn.SWITCH(C14,0,NA(),C14+(RAND()*0.5))</f>
@@ -11334,7 +11326,7 @@
       </c>
       <c r="K14" cm="1">
         <f t="array" aca="1" ref="K14" ca="1">_xlfn.SWITCH(D14,0,NA(),D14+(RAND()*0.5))</f>
-        <v>28.320032432274161</v>
+        <v>28.204713442580633</v>
       </c>
       <c r="L14" t="e" cm="1">
         <f t="array" aca="1" ref="L14" ca="1">_xlfn.SWITCH(E14,0,NA(),E14+(RAND()*0.5))</f>
@@ -11373,7 +11365,7 @@
       </c>
       <c r="I15" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">_xlfn.SWITCH(B15,0,NA(),B15+(RAND()*0.5))</f>
-        <v>31.120431545440891</v>
+        <v>31.416831024138872</v>
       </c>
       <c r="J15" t="e" cm="1">
         <f t="array" aca="1" ref="J15" ca="1">_xlfn.SWITCH(C15,0,NA(),C15+(RAND()*0.5))</f>
@@ -11381,11 +11373,11 @@
       </c>
       <c r="K15" cm="1">
         <f t="array" aca="1" ref="K15" ca="1">_xlfn.SWITCH(D15,0,NA(),D15+(RAND()*0.5))</f>
-        <v>8.3144738602731341</v>
+        <v>8.4530250686686248</v>
       </c>
       <c r="L15" cm="1">
         <f t="array" aca="1" ref="L15" ca="1">_xlfn.SWITCH(E15,0,NA(),E15+(RAND()*0.5))</f>
-        <v>16.304689349326676</v>
+        <v>16.231085208066578</v>
       </c>
       <c r="M15" t="e" cm="1">
         <f t="array" aca="1" ref="M15" ca="1">_xlfn.SWITCH(F15,0,NA(),F15+(RAND()*0.5))</f>
@@ -11420,7 +11412,7 @@
       </c>
       <c r="I16" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">_xlfn.SWITCH(B16,0,NA(),B16+(RAND()*0.5))</f>
-        <v>4.2950394269361505</v>
+        <v>4.4181102579559068</v>
       </c>
       <c r="J16" t="e" cm="1">
         <f t="array" aca="1" ref="J16" ca="1">_xlfn.SWITCH(C16,0,NA(),C16+(RAND()*0.5))</f>
@@ -11467,7 +11459,7 @@
       </c>
       <c r="I17" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">_xlfn.SWITCH(B17,0,NA(),B17+(RAND()*0.5))</f>
-        <v>31.262765653713338</v>
+        <v>31.462421172100999</v>
       </c>
       <c r="J17" t="e" cm="1">
         <f t="array" aca="1" ref="J17" ca="1">_xlfn.SWITCH(C17,0,NA(),C17+(RAND()*0.5))</f>
@@ -11475,7 +11467,7 @@
       </c>
       <c r="K17" cm="1">
         <f t="array" aca="1" ref="K17" ca="1">_xlfn.SWITCH(D17,0,NA(),D17+(RAND()*0.5))</f>
-        <v>26.185310916732359</v>
+        <v>26.123524506294977</v>
       </c>
       <c r="L17" t="e" cm="1">
         <f t="array" aca="1" ref="L17" ca="1">_xlfn.SWITCH(E17,0,NA(),E17+(RAND()*0.5))</f>
@@ -11483,11 +11475,11 @@
       </c>
       <c r="M17" cm="1">
         <f t="array" aca="1" ref="M17" ca="1">_xlfn.SWITCH(F17,0,NA(),F17+(RAND()*0.5))</f>
-        <v>2.0471731212423023</v>
+        <v>2.3614127775548104</v>
       </c>
       <c r="N17" cm="1">
         <f t="array" aca="1" ref="N17" ca="1">_xlfn.SWITCH(G17,0,NA(),G17+(RAND()*0.5))</f>
-        <v>1.0356155504670561</v>
+        <v>1.3977016490040139</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.5">
@@ -11514,7 +11506,7 @@
       </c>
       <c r="I18" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">_xlfn.SWITCH(B18,0,NA(),B18+(RAND()*0.5))</f>
-        <v>31.147550301393355</v>
+        <v>31.440367940564144</v>
       </c>
       <c r="J18" t="e" cm="1">
         <f t="array" aca="1" ref="J18" ca="1">_xlfn.SWITCH(C18,0,NA(),C18+(RAND()*0.5))</f>
@@ -11522,11 +11514,11 @@
       </c>
       <c r="K18" cm="1">
         <f t="array" aca="1" ref="K18" ca="1">_xlfn.SWITCH(D18,0,NA(),D18+(RAND()*0.5))</f>
-        <v>23.467449682996154</v>
+        <v>23.376552979336282</v>
       </c>
       <c r="L18" cm="1">
         <f t="array" aca="1" ref="L18" ca="1">_xlfn.SWITCH(E18,0,NA(),E18+(RAND()*0.5))</f>
-        <v>30.080857493239282</v>
+        <v>30.091086646681312</v>
       </c>
       <c r="M18" t="e" cm="1">
         <f t="array" aca="1" ref="M18" ca="1">_xlfn.SWITCH(F18,0,NA(),F18+(RAND()*0.5))</f>
@@ -11561,7 +11553,7 @@
       </c>
       <c r="I19" cm="1">
         <f t="array" aca="1" ref="I19" ca="1">_xlfn.SWITCH(B19,0,NA(),B19+(RAND()*0.5))</f>
-        <v>31.252320625645694</v>
+        <v>31.369249548056697</v>
       </c>
       <c r="J19" t="e" cm="1">
         <f t="array" aca="1" ref="J19" ca="1">_xlfn.SWITCH(C19,0,NA(),C19+(RAND()*0.5))</f>
@@ -11569,7 +11561,7 @@
       </c>
       <c r="K19" cm="1">
         <f t="array" aca="1" ref="K19" ca="1">_xlfn.SWITCH(D19,0,NA(),D19+(RAND()*0.5))</f>
-        <v>28.378891217076628</v>
+        <v>28.089247940355147</v>
       </c>
       <c r="L19" t="e" cm="1">
         <f t="array" aca="1" ref="L19" ca="1">_xlfn.SWITCH(E19,0,NA(),E19+(RAND()*0.5))</f>
@@ -11608,7 +11600,7 @@
       </c>
       <c r="I20" cm="1">
         <f t="array" aca="1" ref="I20" ca="1">_xlfn.SWITCH(B20,0,NA(),B20+(RAND()*0.5))</f>
-        <v>31.485415094953346</v>
+        <v>31.445192654801264</v>
       </c>
       <c r="J20" t="e" cm="1">
         <f t="array" aca="1" ref="J20" ca="1">_xlfn.SWITCH(C20,0,NA(),C20+(RAND()*0.5))</f>
@@ -11616,15 +11608,15 @@
       </c>
       <c r="K20" cm="1">
         <f t="array" aca="1" ref="K20" ca="1">_xlfn.SWITCH(D20,0,NA(),D20+(RAND()*0.5))</f>
-        <v>5.1317677509213624</v>
+        <v>5.2472909191075097</v>
       </c>
       <c r="L20" cm="1">
         <f t="array" aca="1" ref="L20" ca="1">_xlfn.SWITCH(E20,0,NA(),E20+(RAND()*0.5))</f>
-        <v>31.366307824210971</v>
+        <v>31.379103193205228</v>
       </c>
       <c r="M20" cm="1">
         <f t="array" aca="1" ref="M20" ca="1">_xlfn.SWITCH(F20,0,NA(),F20+(RAND()*0.5))</f>
-        <v>5.322742297855771</v>
+        <v>5.4674717289577455</v>
       </c>
       <c r="N20" t="e" cm="1">
         <f t="array" aca="1" ref="N20" ca="1">_xlfn.SWITCH(G20,0,NA(),G20+(RAND()*0.5))</f>
@@ -11655,7 +11647,7 @@
       </c>
       <c r="I21" cm="1">
         <f t="array" aca="1" ref="I21" ca="1">_xlfn.SWITCH(B21,0,NA(),B21+(RAND()*0.5))</f>
-        <v>31.207700742323802</v>
+        <v>31.456405441568453</v>
       </c>
       <c r="J21" t="e" cm="1">
         <f t="array" aca="1" ref="J21" ca="1">_xlfn.SWITCH(C21,0,NA(),C21+(RAND()*0.5))</f>
@@ -11663,7 +11655,7 @@
       </c>
       <c r="K21" cm="1">
         <f t="array" aca="1" ref="K21" ca="1">_xlfn.SWITCH(D21,0,NA(),D21+(RAND()*0.5))</f>
-        <v>27.045082052367427</v>
+        <v>27.355210351759897</v>
       </c>
       <c r="L21" t="e" cm="1">
         <f t="array" aca="1" ref="L21" ca="1">_xlfn.SWITCH(E21,0,NA(),E21+(RAND()*0.5))</f>
@@ -11702,7 +11694,7 @@
       </c>
       <c r="I22" cm="1">
         <f t="array" aca="1" ref="I22" ca="1">_xlfn.SWITCH(B22,0,NA(),B22+(RAND()*0.5))</f>
-        <v>31.34061826007833</v>
+        <v>31.467108007794707</v>
       </c>
       <c r="J22" t="e" cm="1">
         <f t="array" aca="1" ref="J22" ca="1">_xlfn.SWITCH(C22,0,NA(),C22+(RAND()*0.5))</f>
@@ -11710,11 +11702,11 @@
       </c>
       <c r="K22" cm="1">
         <f t="array" aca="1" ref="K22" ca="1">_xlfn.SWITCH(D22,0,NA(),D22+(RAND()*0.5))</f>
-        <v>31.145459684140935</v>
+        <v>31.492323553978618</v>
       </c>
       <c r="L22" cm="1">
         <f t="array" aca="1" ref="L22" ca="1">_xlfn.SWITCH(E22,0,NA(),E22+(RAND()*0.5))</f>
-        <v>31.291215195525034</v>
+        <v>31.330967765232845</v>
       </c>
       <c r="M22" t="e" cm="1">
         <f t="array" aca="1" ref="M22" ca="1">_xlfn.SWITCH(F22,0,NA(),F22+(RAND()*0.5))</f>
@@ -11749,7 +11741,7 @@
       </c>
       <c r="I23" cm="1">
         <f t="array" aca="1" ref="I23" ca="1">_xlfn.SWITCH(B23,0,NA(),B23+(RAND()*0.5))</f>
-        <v>30.096729792249217</v>
+        <v>30.279329563698237</v>
       </c>
       <c r="J23" t="e" cm="1">
         <f t="array" aca="1" ref="J23" ca="1">_xlfn.SWITCH(C23,0,NA(),C23+(RAND()*0.5))</f>
@@ -11757,15 +11749,15 @@
       </c>
       <c r="K23" cm="1">
         <f t="array" aca="1" ref="K23" ca="1">_xlfn.SWITCH(D23,0,NA(),D23+(RAND()*0.5))</f>
-        <v>26.159040864306363</v>
+        <v>26.219795097284894</v>
       </c>
       <c r="L23" cm="1">
         <f t="array" aca="1" ref="L23" ca="1">_xlfn.SWITCH(E23,0,NA(),E23+(RAND()*0.5))</f>
-        <v>28.233459647030408</v>
+        <v>28.112245651755075</v>
       </c>
       <c r="M23" cm="1">
         <f t="array" aca="1" ref="M23" ca="1">_xlfn.SWITCH(F23,0,NA(),F23+(RAND()*0.5))</f>
-        <v>1.3637677535953165</v>
+        <v>1.0339136295808249</v>
       </c>
       <c r="N23" t="e" cm="1">
         <f t="array" aca="1" ref="N23" ca="1">_xlfn.SWITCH(G23,0,NA(),G23+(RAND()*0.5))</f>
@@ -11796,7 +11788,7 @@
       </c>
       <c r="I24" cm="1">
         <f t="array" aca="1" ref="I24" ca="1">_xlfn.SWITCH(B24,0,NA(),B24+(RAND()*0.5))</f>
-        <v>28.086806403832227</v>
+        <v>28.465298296367251</v>
       </c>
       <c r="J24" t="e" cm="1">
         <f t="array" aca="1" ref="J24" ca="1">_xlfn.SWITCH(C24,0,NA(),C24+(RAND()*0.5))</f>
@@ -11804,11 +11796,11 @@
       </c>
       <c r="K24" cm="1">
         <f t="array" aca="1" ref="K24" ca="1">_xlfn.SWITCH(D24,0,NA(),D24+(RAND()*0.5))</f>
-        <v>18.252188461107949</v>
+        <v>18.031123959078641</v>
       </c>
       <c r="L24" cm="1">
         <f t="array" aca="1" ref="L24" ca="1">_xlfn.SWITCH(E24,0,NA(),E24+(RAND()*0.5))</f>
-        <v>23.482486930823775</v>
+        <v>23.477982785817609</v>
       </c>
       <c r="M24" t="e" cm="1">
         <f t="array" aca="1" ref="M24" ca="1">_xlfn.SWITCH(F24,0,NA(),F24+(RAND()*0.5))</f>
@@ -11843,7 +11835,7 @@
       </c>
       <c r="I25" cm="1">
         <f t="array" aca="1" ref="I25" ca="1">_xlfn.SWITCH(B25,0,NA(),B25+(RAND()*0.5))</f>
-        <v>29.373369342383853</v>
+        <v>29.152605492027078</v>
       </c>
       <c r="J25" t="e" cm="1">
         <f t="array" aca="1" ref="J25" ca="1">_xlfn.SWITCH(C25,0,NA(),C25+(RAND()*0.5))</f>
@@ -11890,19 +11882,19 @@
       </c>
       <c r="I26" cm="1">
         <f t="array" aca="1" ref="I26" ca="1">_xlfn.SWITCH(B26,0,NA(),B26+(RAND()*0.5))</f>
-        <v>26.364594825834761</v>
+        <v>26.441229928225766</v>
       </c>
       <c r="J26" cm="1">
         <f t="array" aca="1" ref="J26" ca="1">_xlfn.SWITCH(C26,0,NA(),C26+(RAND()*0.5))</f>
-        <v>1.1086203324922375</v>
+        <v>1.0862740533764064</v>
       </c>
       <c r="K26" cm="1">
         <f t="array" aca="1" ref="K26" ca="1">_xlfn.SWITCH(D26,0,NA(),D26+(RAND()*0.5))</f>
-        <v>3.3554119889312726</v>
+        <v>3.1012290839292027</v>
       </c>
       <c r="L26" cm="1">
         <f t="array" aca="1" ref="L26" ca="1">_xlfn.SWITCH(E26,0,NA(),E26+(RAND()*0.5))</f>
-        <v>18.098844549609321</v>
+        <v>18.368049572155442</v>
       </c>
       <c r="M26" t="e" cm="1">
         <f t="array" aca="1" ref="M26" ca="1">_xlfn.SWITCH(F26,0,NA(),F26+(RAND()*0.5))</f>
@@ -11937,23 +11929,23 @@
       </c>
       <c r="I27" cm="1">
         <f t="array" aca="1" ref="I27" ca="1">_xlfn.SWITCH(B27,0,NA(),B27+(RAND()*0.5))</f>
-        <v>31.322523796878709</v>
+        <v>31.06776754107883</v>
       </c>
       <c r="J27" cm="1">
         <f t="array" aca="1" ref="J27" ca="1">_xlfn.SWITCH(C27,0,NA(),C27+(RAND()*0.5))</f>
-        <v>3.2863093947018265</v>
+        <v>3.1545694694569439</v>
       </c>
       <c r="K27" cm="1">
         <f t="array" aca="1" ref="K27" ca="1">_xlfn.SWITCH(D27,0,NA(),D27+(RAND()*0.5))</f>
-        <v>31.315025932943279</v>
+        <v>31.205346936651591</v>
       </c>
       <c r="L27" cm="1">
         <f t="array" aca="1" ref="L27" ca="1">_xlfn.SWITCH(E27,0,NA(),E27+(RAND()*0.5))</f>
-        <v>31.49384080281181</v>
+        <v>31.337223247045571</v>
       </c>
       <c r="M27" cm="1">
         <f t="array" aca="1" ref="M27" ca="1">_xlfn.SWITCH(F27,0,NA(),F27+(RAND()*0.5))</f>
-        <v>30.208225990418402</v>
+        <v>30.488210193683983</v>
       </c>
       <c r="N27" t="e" cm="1">
         <f t="array" aca="1" ref="N27" ca="1">_xlfn.SWITCH(G27,0,NA(),G27+(RAND()*0.5))</f>
@@ -11984,19 +11976,19 @@
       </c>
       <c r="I28" cm="1">
         <f t="array" aca="1" ref="I28" ca="1">_xlfn.SWITCH(B28,0,NA(),B28+(RAND()*0.5))</f>
-        <v>26.036942692492595</v>
+        <v>26.138725705630371</v>
       </c>
       <c r="J28" cm="1">
         <f t="array" aca="1" ref="J28" ca="1">_xlfn.SWITCH(C28,0,NA(),C28+(RAND()*0.5))</f>
-        <v>12.272374383789597</v>
+        <v>12.43685809570859</v>
       </c>
       <c r="K28" cm="1">
         <f t="array" aca="1" ref="K28" ca="1">_xlfn.SWITCH(D28,0,NA(),D28+(RAND()*0.5))</f>
-        <v>2.4456348089841082</v>
+        <v>2.3419397129491037</v>
       </c>
       <c r="L28" cm="1">
         <f t="array" aca="1" ref="L28" ca="1">_xlfn.SWITCH(E28,0,NA(),E28+(RAND()*0.5))</f>
-        <v>24.300379063965124</v>
+        <v>24.114409142835832</v>
       </c>
       <c r="M28" t="e" cm="1">
         <f t="array" aca="1" ref="M28" ca="1">_xlfn.SWITCH(F28,0,NA(),F28+(RAND()*0.5))</f>
@@ -12031,7 +12023,7 @@
       </c>
       <c r="I29" cm="1">
         <f t="array" aca="1" ref="I29" ca="1">_xlfn.SWITCH(B29,0,NA(),B29+(RAND()*0.5))</f>
-        <v>31.207941650955885</v>
+        <v>31.050714405600107</v>
       </c>
       <c r="J29" t="e" cm="1">
         <f t="array" aca="1" ref="J29" ca="1">_xlfn.SWITCH(C29,0,NA(),C29+(RAND()*0.5))</f>
@@ -12039,7 +12031,7 @@
       </c>
       <c r="K29" cm="1">
         <f t="array" aca="1" ref="K29" ca="1">_xlfn.SWITCH(D29,0,NA(),D29+(RAND()*0.5))</f>
-        <v>24.460683513794638</v>
+        <v>24.460721535470892</v>
       </c>
       <c r="L29" t="e" cm="1">
         <f t="array" aca="1" ref="L29" ca="1">_xlfn.SWITCH(E29,0,NA(),E29+(RAND()*0.5))</f>
@@ -12078,7 +12070,7 @@
       </c>
       <c r="I30" cm="1">
         <f t="array" aca="1" ref="I30" ca="1">_xlfn.SWITCH(B30,0,NA(),B30+(RAND()*0.5))</f>
-        <v>31.279108116327787</v>
+        <v>31.199354490885145</v>
       </c>
       <c r="J30" t="e" cm="1">
         <f t="array" aca="1" ref="J30" ca="1">_xlfn.SWITCH(C30,0,NA(),C30+(RAND()*0.5))</f>
@@ -12086,7 +12078,7 @@
       </c>
       <c r="K30" cm="1">
         <f t="array" aca="1" ref="K30" ca="1">_xlfn.SWITCH(D30,0,NA(),D30+(RAND()*0.5))</f>
-        <v>3.272083564260468</v>
+        <v>3.3481777610121606</v>
       </c>
       <c r="L30" t="e" cm="1">
         <f t="array" aca="1" ref="L30" ca="1">_xlfn.SWITCH(E30,0,NA(),E30+(RAND()*0.5))</f>
@@ -12125,7 +12117,7 @@
       </c>
       <c r="I31" cm="1">
         <f t="array" aca="1" ref="I31" ca="1">_xlfn.SWITCH(B31,0,NA(),B31+(RAND()*0.5))</f>
-        <v>19.401169814586368</v>
+        <v>19.158111593861499</v>
       </c>
       <c r="J31" t="e" cm="1">
         <f t="array" aca="1" ref="J31" ca="1">_xlfn.SWITCH(C31,0,NA(),C31+(RAND()*0.5))</f>
@@ -12172,15 +12164,15 @@
       </c>
       <c r="I32" cm="1">
         <f t="array" aca="1" ref="I32" ca="1">_xlfn.SWITCH(B32,0,NA(),B32+(RAND()*0.5))</f>
-        <v>31.351263915361923</v>
+        <v>31.439357081533554</v>
       </c>
       <c r="J32" cm="1">
         <f t="array" aca="1" ref="J32" ca="1">_xlfn.SWITCH(C32,0,NA(),C32+(RAND()*0.5))</f>
-        <v>16.352985599826461</v>
+        <v>16.317198288191733</v>
       </c>
       <c r="K32" cm="1">
         <f t="array" aca="1" ref="K32" ca="1">_xlfn.SWITCH(D32,0,NA(),D32+(RAND()*0.5))</f>
-        <v>31.255659209738887</v>
+        <v>31.060873735585556</v>
       </c>
       <c r="L32" t="e" cm="1">
         <f t="array" aca="1" ref="L32" ca="1">_xlfn.SWITCH(E32,0,NA(),E32+(RAND()*0.5))</f>
@@ -12219,7 +12211,7 @@
       </c>
       <c r="I33" cm="1">
         <f t="array" aca="1" ref="I33" ca="1">_xlfn.SWITCH(B33,0,NA(),B33+(RAND()*0.5))</f>
-        <v>31.339769137303353</v>
+        <v>31.467372477214536</v>
       </c>
       <c r="J33" t="e" cm="1">
         <f t="array" aca="1" ref="J33" ca="1">_xlfn.SWITCH(C33,0,NA(),C33+(RAND()*0.5))</f>
@@ -12266,7 +12258,7 @@
       </c>
       <c r="I34" cm="1">
         <f t="array" aca="1" ref="I34" ca="1">_xlfn.SWITCH(B34,0,NA(),B34+(RAND()*0.5))</f>
-        <v>29.125343932455021</v>
+        <v>29.279239435850442</v>
       </c>
       <c r="J34" t="e" cm="1">
         <f t="array" aca="1" ref="J34" ca="1">_xlfn.SWITCH(C34,0,NA(),C34+(RAND()*0.5))</f>
@@ -12274,11 +12266,11 @@
       </c>
       <c r="K34" cm="1">
         <f t="array" aca="1" ref="K34" ca="1">_xlfn.SWITCH(D34,0,NA(),D34+(RAND()*0.5))</f>
-        <v>15.166878785367489</v>
+        <v>15.117989060446702</v>
       </c>
       <c r="L34" cm="1">
         <f t="array" aca="1" ref="L34" ca="1">_xlfn.SWITCH(E34,0,NA(),E34+(RAND()*0.5))</f>
-        <v>18.005857944050817</v>
+        <v>18.084431201653999</v>
       </c>
       <c r="M34" t="e" cm="1">
         <f t="array" aca="1" ref="M34" ca="1">_xlfn.SWITCH(F34,0,NA(),F34+(RAND()*0.5))</f>
@@ -12313,7 +12305,7 @@
       </c>
       <c r="I35" cm="1">
         <f t="array" aca="1" ref="I35" ca="1">_xlfn.SWITCH(B35,0,NA(),B35+(RAND()*0.5))</f>
-        <v>31.32400601742998</v>
+        <v>31.102067177685047</v>
       </c>
       <c r="J35" t="e" cm="1">
         <f t="array" aca="1" ref="J35" ca="1">_xlfn.SWITCH(C35,0,NA(),C35+(RAND()*0.5))</f>
@@ -12325,11 +12317,11 @@
       </c>
       <c r="L35" cm="1">
         <f t="array" aca="1" ref="L35" ca="1">_xlfn.SWITCH(E35,0,NA(),E35+(RAND()*0.5))</f>
-        <v>31.259716430408627</v>
+        <v>31.409788815201715</v>
       </c>
       <c r="M35" cm="1">
         <f t="array" aca="1" ref="M35" ca="1">_xlfn.SWITCH(F35,0,NA(),F35+(RAND()*0.5))</f>
-        <v>24.086040676067817</v>
+        <v>24.182463286258006</v>
       </c>
       <c r="N35" t="e" cm="1">
         <f t="array" aca="1" ref="N35" ca="1">_xlfn.SWITCH(G35,0,NA(),G35+(RAND()*0.5))</f>
@@ -12407,115 +12399,126 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D65371F-9363-48D7-BA63-4E2E6AC685C9}">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:O37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="10.76171875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.6">
-      <c r="A1" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="47" t="s">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.6">
+      <c r="B1" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
+      <c r="J1" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
     </row>
-    <row r="2" spans="1:14" ht="43" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
+    <row r="2" spans="1:15" ht="43" x14ac:dyDescent="0.5">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="3"/>
+      <c r="J2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>54</v>
+      <c r="O2" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3">
+        <v>1503960366</v>
+      </c>
+      <c r="B3">
         <v>31</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>25</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
       <c r="E3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>31</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>16</v>
-      </c>
-      <c r="K3">
-        <v>31</v>
       </c>
       <c r="L3">
         <v>31</v>
       </c>
       <c r="M3">
+        <v>31</v>
+      </c>
+      <c r="N3">
         <v>30</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4">
+        <v>1624580081</v>
+      </c>
+      <c r="B4">
         <v>31</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
       <c r="C4">
         <v>0</v>
       </c>
@@ -12531,38 +12534,41 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>31</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>12</v>
-      </c>
-      <c r="K4">
-        <v>31</v>
       </c>
       <c r="L4">
         <v>31</v>
       </c>
       <c r="M4">
+        <v>31</v>
+      </c>
+      <c r="N4">
         <v>24</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A5">
+        <v>1644430081</v>
+      </c>
+      <c r="B5">
         <v>30</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
       <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
       <c r="E5">
         <v>0</v>
       </c>
@@ -12572,38 +12578,41 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <v>31</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>3</v>
-      </c>
-      <c r="K5">
-        <v>31</v>
       </c>
       <c r="L5">
         <v>31</v>
       </c>
       <c r="M5">
+        <v>31</v>
+      </c>
+      <c r="N5">
         <v>5</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6">
+        <v>1844505072</v>
+      </c>
+      <c r="B6">
         <v>31</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
       <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>3</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
       <c r="E6">
         <v>0</v>
       </c>
@@ -12613,161 +12622,173 @@
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="J6">
         <v>31</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>1</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>28</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>31</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>2</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A7">
+        <v>1927972279</v>
+      </c>
+      <c r="B7">
         <v>31</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
       <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>5</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="J7">
         <v>31</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
       <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
         <v>28</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>31</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>2</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A8">
+        <v>2022484408</v>
+      </c>
+      <c r="B8">
         <v>31</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
         <v>31</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="I8">
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="J8">
         <v>31</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
       <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
         <v>28</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>30</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>2</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A9">
+        <v>2026352035</v>
+      </c>
+      <c r="B9">
         <v>31</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
       <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
         <v>28</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>4</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="I9">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="J9">
         <v>31</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
       <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
         <v>27</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>28</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>1</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A10">
+        <v>2320127002</v>
+      </c>
+      <c r="B10">
         <v>31</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
       <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
         <v>1</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
       <c r="E10">
         <v>0</v>
       </c>
@@ -12777,73 +12798,79 @@
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="J10">
         <v>31</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
       <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
         <v>26</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>24</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>1</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A11">
+        <v>2347167796</v>
+      </c>
+      <c r="B11">
         <v>18</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
       <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
         <v>15</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>18</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="I11">
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="J11">
         <v>31</v>
       </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
       <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
         <v>26</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>23</v>
       </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
       <c r="N11">
         <v>0</v>
       </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A12">
+        <v>2873212765</v>
+      </c>
+      <c r="B12">
         <v>31</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
       <c r="C12">
         <v>0</v>
       </c>
@@ -12851,40 +12878,43 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="J12">
         <v>31</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
       <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
         <v>25</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>18</v>
       </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
       <c r="N12">
         <v>0</v>
       </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A13">
+        <v>3372868164</v>
+      </c>
+      <c r="B13">
         <v>20</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
       <c r="C13">
         <v>0</v>
       </c>
@@ -12900,38 +12930,41 @@
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="I13">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="J13">
         <v>31</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
       <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
         <v>24</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>18</v>
       </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
       <c r="N13">
         <v>0</v>
       </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A14">
+        <v>3977333714</v>
+      </c>
+      <c r="B14">
         <v>30</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
       <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
         <v>28</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
       <c r="E14">
         <v>0</v>
       </c>
@@ -12941,73 +12974,79 @@
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="I14">
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="J14">
         <v>31</v>
       </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
       <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
         <v>23</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>18</v>
       </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
       <c r="N14">
         <v>0</v>
       </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A15">
+        <v>4020332650</v>
+      </c>
+      <c r="B15">
         <v>31</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
       <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
         <v>8</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>16</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
-      <c r="I15">
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="J15">
         <v>31</v>
       </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
       <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
         <v>18</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>16</v>
       </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
       <c r="N15">
         <v>0</v>
       </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A16">
+        <v>4057192912</v>
+      </c>
+      <c r="B16">
         <v>4</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
       <c r="C16">
         <v>0</v>
       </c>
@@ -13023,120 +13062,129 @@
       <c r="G16">
         <v>0</v>
       </c>
-      <c r="I16">
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="J16">
         <v>31</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
       <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
         <v>15</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>4</v>
       </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
       <c r="N16">
         <v>0</v>
       </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A17">
+        <v>4319703577</v>
+      </c>
+      <c r="B17">
         <v>31</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
       <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
         <v>26</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
       <c r="E17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
       <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>31</v>
       </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
       <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
         <v>15</v>
       </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17">
         <v>0</v>
       </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A18">
+        <v>4388161847</v>
+      </c>
+      <c r="B18">
         <v>31</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
       <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
         <v>23</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>30</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
-      <c r="I18">
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="J18">
         <v>31</v>
       </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
       <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
         <v>8</v>
       </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="N18">
         <v>0</v>
       </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A19">
+        <v>4445114986</v>
+      </c>
+      <c r="B19">
         <v>31</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
       <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
         <v>28</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
       <c r="E19">
         <v>0</v>
       </c>
@@ -13146,79 +13194,85 @@
       <c r="G19">
         <v>0</v>
       </c>
-      <c r="I19">
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="J19">
         <v>31</v>
       </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
       <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
         <v>5</v>
       </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
       <c r="M19">
         <v>0</v>
       </c>
       <c r="N19">
         <v>0</v>
       </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A20">
+        <v>4558609924</v>
+      </c>
+      <c r="B20">
         <v>31</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
       <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
         <v>5</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>31</v>
-      </c>
-      <c r="E20">
-        <v>5</v>
       </c>
       <c r="F20">
         <v>5</v>
       </c>
       <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="I20">
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="J20">
         <v>31</v>
       </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
       <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
         <v>5</v>
       </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20">
         <v>0</v>
       </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A21">
+        <v>4702921684</v>
+      </c>
+      <c r="B21">
         <v>31</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
       <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
         <v>27</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
       <c r="E21">
         <v>0</v>
       </c>
@@ -13228,40 +13282,43 @@
       <c r="G21">
         <v>0</v>
       </c>
-      <c r="I21">
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="J21">
         <v>31</v>
       </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
       <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
         <v>4</v>
       </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21">
         <v>0</v>
       </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A22">
+        <v>5553957443</v>
+      </c>
+      <c r="B22">
         <v>31</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
       <c r="C22">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="D22">
         <v>31</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -13269,114 +13326,123 @@
       <c r="G22">
         <v>0</v>
       </c>
-      <c r="I22">
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="J22">
         <v>31</v>
       </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
       <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
         <v>3</v>
       </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
       <c r="M22">
         <v>0</v>
       </c>
       <c r="N22">
         <v>0</v>
       </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A23">
+        <v>5577150313</v>
+      </c>
+      <c r="B23">
         <v>30</v>
       </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
       <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
         <v>26</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>28</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="J23">
         <v>31</v>
       </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
       <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
         <v>3</v>
       </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
       <c r="M23">
         <v>0</v>
       </c>
       <c r="N23">
         <v>0</v>
       </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A24">
+        <v>6117666160</v>
+      </c>
+      <c r="B24">
         <v>28</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
       <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
         <v>18</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>23</v>
       </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
-      <c r="I24">
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="J24">
         <v>30</v>
       </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
       <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
         <v>3</v>
       </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
       <c r="M24">
         <v>0</v>
       </c>
       <c r="N24">
         <v>0</v>
       </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A25">
+        <v>6290855005</v>
+      </c>
+      <c r="B25">
         <v>29</v>
       </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
       <c r="C25">
         <v>0</v>
       </c>
@@ -13392,94 +13458,100 @@
       <c r="G25">
         <v>0</v>
       </c>
-      <c r="I25">
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="J25">
         <v>30</v>
       </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
       <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
         <v>2</v>
       </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
       <c r="M25">
         <v>0</v>
       </c>
       <c r="N25">
         <v>0</v>
       </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A26">
+        <v>6775888955</v>
+      </c>
+      <c r="B26">
         <v>26</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>1</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>3</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>18</v>
       </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
-      <c r="I26">
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="J26">
         <v>30</v>
       </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
       <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
         <v>1</v>
       </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
       <c r="M26">
         <v>0</v>
       </c>
       <c r="N26">
         <v>0</v>
       </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A27">
+        <v>6962181067</v>
+      </c>
+      <c r="B27">
         <v>31</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>3</v>
-      </c>
-      <c r="C27">
-        <v>31</v>
       </c>
       <c r="D27">
         <v>31</v>
       </c>
       <c r="E27">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F27">
         <v>30</v>
       </c>
       <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="I27">
+        <v>30</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="J27">
         <v>29</v>
       </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
       <c r="K27">
         <v>0</v>
       </c>
@@ -13492,35 +13564,38 @@
       <c r="N27">
         <v>0</v>
       </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A28">
+        <v>7007744171</v>
+      </c>
+      <c r="B28">
         <v>26</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>12</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>2</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>24</v>
       </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
-      <c r="I28">
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="J28">
         <v>29</v>
       </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
       <c r="K28">
         <v>0</v>
       </c>
@@ -13533,20 +13608,23 @@
       <c r="N28">
         <v>0</v>
       </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A29">
+        <v>7086361926</v>
+      </c>
+      <c r="B29">
         <v>31</v>
       </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
       <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
         <v>24</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
       <c r="E29">
         <v>0</v>
       </c>
@@ -13556,12 +13634,12 @@
       <c r="G29">
         <v>0</v>
       </c>
-      <c r="I29">
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="J29">
         <v>28</v>
       </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
       <c r="K29">
         <v>0</v>
       </c>
@@ -13574,20 +13652,23 @@
       <c r="N29">
         <v>0</v>
       </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A30">
+        <v>8053475328</v>
+      </c>
+      <c r="B30">
         <v>31</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
       <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
         <v>3</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
       <c r="E30">
         <v>0</v>
       </c>
@@ -13597,12 +13678,12 @@
       <c r="G30">
         <v>0</v>
       </c>
-      <c r="I30">
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="J30">
         <v>26</v>
       </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
       <c r="K30">
         <v>0</v>
       </c>
@@ -13615,14 +13696,17 @@
       <c r="N30">
         <v>0</v>
       </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A31">
+        <v>8253242879</v>
+      </c>
+      <c r="B31">
         <v>19</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
       <c r="C31">
         <v>0</v>
       </c>
@@ -13638,12 +13722,12 @@
       <c r="G31">
         <v>0</v>
       </c>
-      <c r="I31">
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="J31">
         <v>26</v>
       </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
       <c r="K31">
         <v>0</v>
       </c>
@@ -13656,20 +13740,23 @@
       <c r="N31">
         <v>0</v>
       </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A32">
+        <v>8378563200</v>
+      </c>
+      <c r="B32">
         <v>31</v>
       </c>
-      <c r="B32">
+      <c r="C32">
         <v>16</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>31</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
       <c r="E32">
         <v>0</v>
       </c>
@@ -13679,12 +13766,12 @@
       <c r="G32">
         <v>0</v>
       </c>
-      <c r="I32">
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="J32">
         <v>20</v>
       </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
       <c r="K32">
         <v>0</v>
       </c>
@@ -13697,14 +13784,17 @@
       <c r="N32">
         <v>0</v>
       </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A33">
+        <v>8583815059</v>
+      </c>
+      <c r="B33">
         <v>31</v>
       </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
       <c r="C33">
         <v>0</v>
       </c>
@@ -13720,12 +13810,12 @@
       <c r="G33">
         <v>0</v>
       </c>
-      <c r="I33">
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="J33">
         <v>19</v>
       </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
       <c r="K33">
         <v>0</v>
       </c>
@@ -13738,35 +13828,38 @@
       <c r="N33">
         <v>0</v>
       </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A34">
+        <v>8792009665</v>
+      </c>
+      <c r="B34">
         <v>29</v>
       </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
       <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
         <v>15</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>18</v>
       </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
       <c r="F34">
         <v>0</v>
       </c>
       <c r="G34">
         <v>0</v>
       </c>
-      <c r="I34">
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="J34">
         <v>18</v>
       </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
       <c r="K34">
         <v>0</v>
       </c>
@@ -13779,35 +13872,38 @@
       <c r="N34">
         <v>0</v>
       </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A35">
+        <v>8877689391</v>
+      </c>
+      <c r="B35">
         <v>31</v>
       </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
         <v>31</v>
-      </c>
-      <c r="E35">
-        <v>24</v>
       </c>
       <c r="F35">
         <v>24</v>
       </c>
       <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="I35">
+        <v>24</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="J35">
         <v>4</v>
       </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
       <c r="K35">
         <v>0</v>
       </c>
@@ -13820,31 +13916,52 @@
       <c r="N35">
         <v>0</v>
       </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.5">
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="J36" s="41"/>
+      <c r="K36" s="41"/>
+      <c r="L36" s="41"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="41"/>
+      <c r="O36" s="41"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.5">
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45"/>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="J37">
+        <f>SUM(J2:J35)</f>
+        <v>940</v>
+      </c>
+      <c r="K37">
+        <f t="shared" ref="K37:O37" si="0">SUM(K2:K35)</f>
+        <v>32</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="0"/>
+        <v>410</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="0"/>
+        <v>334</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N3:N35">
-    <sortCondition descending="1" ref="N3:N35"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O3:O35">
+    <sortCondition descending="1" ref="O3:O35"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="J1:O1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:G35">
+  <conditionalFormatting sqref="B3:H35">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -13866,7 +13983,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:G37">
+  <conditionalFormatting sqref="B3:H37">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -13886,7 +14003,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:N35">
+  <conditionalFormatting sqref="J3:O35">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -13926,7 +14043,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36:N37">
+  <conditionalFormatting sqref="J36:O36">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>